<commit_message>
updated list of bugs
</commit_message>
<xml_diff>
--- a/GameplayBugs.xlsx
+++ b/GameplayBugs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Header</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Projectile: If enemy is too close it do not hit it</t>
+  </si>
+  <si>
+    <t>BlockMove - Animation could not found at assassine</t>
+  </si>
+  <si>
+    <t>get stunned while in air --&gt; slow fall</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,6 +404,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed issues from Bug-List
- sliding in die animation when killed in air or with knockback
- get stunned while in air --> slow fall
- BlockMove - Animation could not found at assassine
</commit_message>
<xml_diff>
--- a/GameplayBugs.xlsx
+++ b/GameplayBugs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Header</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Other actions while dashing are possible</t>
   </si>
   <si>
-    <t>Not Fixed</t>
-  </si>
-  <si>
     <t>First Frame of Animation is wrong</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>Sandro</t>
+  </si>
+  <si>
+    <t>Sliding in die animation when killed in air or with knockback</t>
   </si>
 </sst>
 </file>
@@ -384,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -404,15 +404,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -420,45 +423,65 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>